<commit_message>
fear: updated the test plan
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CUBoulder\PES\Project\Bootloader_git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696F6172-D0BC-4844-8B3B-73FFE8768247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E844A72E-027F-4B2B-B6A5-729CA6AE7328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{38B7B26A-E2A4-41D8-AEA1-564DC2CBD083}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
   <si>
     <t>Title</t>
   </si>
@@ -49,9 +49,6 @@
     <t>PASS/FAIL</t>
   </si>
   <si>
-    <t>Timestamp</t>
-  </si>
-  <si>
     <t>Manual Test Case Plan for PES Project: Bootloader</t>
   </si>
   <si>
@@ -106,15 +103,9 @@
     <t>Firmware verification</t>
   </si>
   <si>
-    <t>When the user presses the boot command and if the firmware is present then the code checks and boots the app without the issuing a fault</t>
-  </si>
-  <si>
     <t>No errors printed, the verification signature is correct.</t>
   </si>
   <si>
-    <t>When the user presses the boot command and if the firmware is not present then the code checks and prints error</t>
-  </si>
-  <si>
     <t>No error should be printed</t>
   </si>
   <si>
@@ -136,9 +127,6 @@
     <t>Application boots up if no input is provided.</t>
   </si>
   <si>
-    <t>Green LED should be blinking whenever in the bootloader mode</t>
-  </si>
-  <si>
     <t>Green LED blinks in the bootloader mode</t>
   </si>
   <si>
@@ -160,23 +148,116 @@
     <t>Prints the error</t>
   </si>
   <si>
-    <t>Flash should not write in bootloader region</t>
-  </si>
-  <si>
-    <t>Flash should not write in invalid location</t>
-  </si>
-  <si>
     <t>Prints error and Blink Red LED</t>
   </si>
   <si>
     <t>Prints the error and RED LED blinks.</t>
+  </si>
+  <si>
+    <t>Step Performed</t>
+  </si>
+  <si>
+    <t>1. Plug the USB.
+2. Wait for the 20 second timeout.
+3. The program should boot up automatically</t>
+  </si>
+  <si>
+    <t>1. Plug the USB.
+2. Enter the erase command and hit enter.
+3. No error should be printed</t>
+  </si>
+  <si>
+    <t>1. Plug the USB.
+2. Enter the erase command and hit enter.
+3. No error should be printed
+4. Enter the prog coomand and hit enter.
+5. The systems should be waiting for data.</t>
+  </si>
+  <si>
+    <t>1. Plug the USB.
+2. Enter the erase command and hit enter.
+3. No error should be printed
+4. Enter the prog coomand and hit enter.
+5. The systems should be waiting for data.
+6. Tera Term: File-&gt;Send File-&gt;Select the .s19 file
+7. Transfer should begin.
+8. Bootloader should boot the image successfully.</t>
+  </si>
+  <si>
+    <t>When the user presses the boot command and if the firmware is present and the verification signature is written then the bootloader boots the new app without the issuing a fault</t>
+  </si>
+  <si>
+    <t>1. Plug in the USB.
+2. Enter the boot command and hit enter.</t>
+  </si>
+  <si>
+    <t>When the user presses the boot command and if the firmware is not present and the verification signature is not written then the bootloader prints an error.</t>
+  </si>
+  <si>
+    <t>1. Plug the USB.</t>
+  </si>
+  <si>
+    <t>Green LED should be blinking in the bootloader mode</t>
+  </si>
+  <si>
+    <t>1. Plug the USB.
+2. Enter an invalid command and hit enter.</t>
+  </si>
+  <si>
+    <t>Flash should not write in an invalid location</t>
+  </si>
+  <si>
+    <t>The firmware file should not contain the flash region to be modified that belongs to the bootloader otherwise that could cause bootloader corruption potentially bricking the device.</t>
+  </si>
+  <si>
+    <t>Sankalp Agrawal
+11-12-2021</t>
+  </si>
+  <si>
+    <t>Sankalp Agrawal
+11-12-2022</t>
+  </si>
+  <si>
+    <t>Sankalp Agrawal
+11-12-2023</t>
+  </si>
+  <si>
+    <t>Sankalp Agrawal
+11-12-2024</t>
+  </si>
+  <si>
+    <t>Sankalp Agrawal
+11-12-2025</t>
+  </si>
+  <si>
+    <t>Sankalp Agrawal
+11-12-2026</t>
+  </si>
+  <si>
+    <t>Sankalp Agrawal
+11-12-2027</t>
+  </si>
+  <si>
+    <t>Sankalp Agrawal
+11-12-2028</t>
+  </si>
+  <si>
+    <t>Sankalp Agrawal
+11-12-2029</t>
+  </si>
+  <si>
+    <t>Sankalp Agrawal
+11-12-2030</t>
+  </si>
+  <si>
+    <t>Tester/Timestamp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +268,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -567,40 +654,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B749583-AF9F-4EE9-B6E8-5C39159FA5F2}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.6328125" style="1" customWidth="1"/>
-    <col min="2" max="4" width="17.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6328125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="2" max="3" width="17.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6328125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -611,179 +702,233 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="G4" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="3"/>
+      <c r="G5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="F6" s="3"/>
+      <c r="G6" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="F7" s="3"/>
+      <c r="G7" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="F8" s="3"/>
+      <c r="G8" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="174" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="F9" s="3"/>
+      <c r="G9" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="D11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="F11" s="3"/>
+      <c r="G11" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="F12" s="3"/>
+      <c r="G12" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="F13" s="3"/>
+      <c r="G13" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="D14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A1:G2"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>